<commit_message>
Criação do menu inicial e ajustes de salto do player 1
</commit_message>
<xml_diff>
--- a/tab.xlsx
+++ b/tab.xlsx
@@ -720,7 +720,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -728,8 +728,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -738,7 +745,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -770,10 +789,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1057,7 +1077,7 @@
   <dimension ref="A1:T12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1068,31 +1088,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -1101,28 +1121,28 @@
       <c r="K1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="3" t="s">
         <v>27</v>
       </c>
       <c r="T1" s="1" t="s">
@@ -1130,31 +1150,31 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="J2" s="2" t="s">
@@ -1163,25 +1183,25 @@
       <c r="K2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="Q2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="R2" s="3" t="s">
         <v>47</v>
       </c>
       <c r="S2" s="1" t="s">
@@ -1192,31 +1212,31 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="2" t="s">
         <v>38</v>
       </c>
       <c r="J3" s="2" t="s">
@@ -1225,22 +1245,22 @@
       <c r="K3" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="N3" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="O3" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="P3" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" s="3" t="s">
         <v>56</v>
       </c>
       <c r="R3" s="1" t="s">
@@ -1254,31 +1274,31 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="2" t="s">
         <v>75</v>
       </c>
       <c r="J4" s="2" t="s">
@@ -1287,19 +1307,19 @@
       <c r="K4" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="M4" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="N4" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="O4" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="P4" s="3" t="s">
         <v>82</v>
       </c>
       <c r="Q4" s="1" t="s">
@@ -1316,31 +1336,31 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="2" t="s">
         <v>94</v>
       </c>
       <c r="J5" s="2" t="s">
@@ -1349,16 +1369,16 @@
       <c r="K5" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="L5" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="M5" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="N5" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="O5" s="2" t="s">
         <v>100</v>
       </c>
       <c r="P5" s="1" t="s">
@@ -1378,46 +1398,46 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="L6" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="M6" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="N6" s="3" t="s">
         <v>118</v>
       </c>
       <c r="O6" s="1" t="s">
@@ -1440,43 +1460,43 @@
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="L7" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="M7" s="3" t="s">
         <v>136</v>
       </c>
       <c r="N7" s="1" t="s">
@@ -1502,19 +1522,19 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>147</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -1529,10 +1549,10 @@
       <c r="I8" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="K8" s="1" t="s">
         <v>153</v>
       </c>
       <c r="L8" s="1" t="s">
@@ -1564,25 +1584,25 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="3" t="s">
         <v>168</v>
       </c>
       <c r="H9" s="1" t="s">
@@ -1591,10 +1611,10 @@
       <c r="I9" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="K9" s="1" t="s">
         <v>172</v>
       </c>
       <c r="L9" s="1" t="s">
@@ -1626,25 +1646,25 @@
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="3" t="s">
         <v>187</v>
       </c>
       <c r="H10" s="1" t="s">
@@ -1653,10 +1673,10 @@
       <c r="I10" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="K10" s="1" t="s">
         <v>191</v>
       </c>
       <c r="L10" s="1" t="s">
@@ -1688,37 +1708,37 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="K11" s="1" t="s">
         <v>210</v>
       </c>
       <c r="L11" s="1" t="s">
@@ -1750,37 +1770,37 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" s="3" t="s">
         <v>47</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="K12" s="1" t="s">
         <v>220</v>
       </c>
       <c r="L12" s="1" t="s">
@@ -1813,5 +1833,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>